<commit_message>
update ChooseItemManager load sprite to game
</commit_message>
<xml_diff>
--- a/MySurvivorsGame/Assets/StreamingAssets/WeaponData.xlsx
+++ b/MySurvivorsGame/Assets/StreamingAssets/WeaponData.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
   <si>
     <t>WeaponName</t>
   </si>
@@ -26,6 +26,12 @@
     <t>NowWeaponLevel</t>
   </si>
   <si>
+    <t>UIPath</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
     <t>武器名稱</t>
   </si>
   <si>
@@ -38,6 +44,12 @@
     <t>現在武器階段</t>
   </si>
   <si>
+    <t>武器UI路徑</t>
+  </si>
+  <si>
+    <t>武器說明</t>
+  </si>
+  <si>
     <t>string</t>
   </si>
   <si>
@@ -48,6 +60,12 @@
   </si>
   <si>
     <t>Assets/Prefabs/Weapons/Dark Magic.prefab</t>
+  </si>
+  <si>
+    <t>Assets/ArtResources/Weapons/Weapons Sprite Sheet.png[Weapons Sprite Sheet_123]</t>
+  </si>
+  <si>
+    <t>朝向の方向に素早く発射します</t>
   </si>
   <si>
     <t>Level</t>
@@ -353,6 +371,8 @@
     <col customWidth="1" min="2" max="2" width="36.75"/>
     <col customWidth="1" min="3" max="3" width="16.5"/>
     <col customWidth="1" min="4" max="4" width="18.5"/>
+    <col customWidth="1" min="5" max="5" width="67.0"/>
+    <col customWidth="1" min="6" max="6" width="26.63"/>
     <col customWidth="1" min="11" max="11" width="15.25"/>
   </cols>
   <sheetData>
@@ -369,22 +389,32 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
+        <v>9</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -392,19 +422,23 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
+        <v>13</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
@@ -412,19 +446,23 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D4" s="2">
         <v>1.0</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -450,62 +488,62 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
update unity add fireball to data
</commit_message>
<xml_diff>
--- a/MySurvivorsGame/Assets/StreamingAssets/WeaponData.xlsx
+++ b/MySurvivorsGame/Assets/StreamingAssets/WeaponData.xlsx
@@ -5,6 +5,7 @@
   <sheets>
     <sheet state="visible" name="WeaponData" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="MagicBall" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="FireBall" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="42">
   <si>
     <t>WeaponName</t>
   </si>
@@ -84,6 +85,21 @@
   </si>
   <si>
     <t>MagicBallController</t>
+  </si>
+  <si>
+    <t>FireBall</t>
+  </si>
+  <si>
+    <t>Assets/Prefabs/Weapons/FireBall.prefab</t>
+  </si>
+  <si>
+    <t>Assets/ArtResources/Weapons/RotateFire/Effect3/1.png</t>
+  </si>
+  <si>
+    <t>周囲を回転しながら攻撃します。</t>
+  </si>
+  <si>
+    <t>FireBallController</t>
   </si>
   <si>
     <t>Level</t>
@@ -179,6 +195,10 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -489,7 +509,7 @@
         <v>18</v>
       </c>
       <c r="D4" s="2">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>20</v>
@@ -507,12 +527,30 @@
       <c r="J4" s="2"/>
     </row>
     <row r="5">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
+      <c r="A5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2"/>
@@ -542,42 +580,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3">
@@ -585,19 +623,19 @@
         <v>17</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4">
@@ -678,6 +716,164 @@
       </c>
       <c r="F7" s="2">
         <v>7.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="5" max="5" width="11.5"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="B4" s="2">
+        <v>10.0</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E4" s="2">
+        <v>10.0</v>
+      </c>
+      <c r="F4" s="2">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="B5" s="2">
+        <v>10.0</v>
+      </c>
+      <c r="C5" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="D5" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="E5" s="2">
+        <v>11.5</v>
+      </c>
+      <c r="F5" s="2">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="B6" s="2">
+        <v>40.0</v>
+      </c>
+      <c r="C6" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="D6" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="E6" s="2">
+        <v>13.0</v>
+      </c>
+      <c r="F6" s="2">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="B7" s="2">
+        <v>60.0</v>
+      </c>
+      <c r="C7" s="2">
+        <v>5.0</v>
+      </c>
+      <c r="D7" s="2">
+        <v>8.0</v>
+      </c>
+      <c r="E7" s="2">
+        <v>14.5</v>
+      </c>
+      <c r="F7" s="2">
+        <v>12.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>